<commit_message>
add 7 more properties (matchday, season, matchname, hometeam, guestteam, hometeam_cn, guestteam_cn) into EuroOdds. MatchEuroOdds will not be used
</commit_message>
<xml_diff>
--- a/sportsbook/sportsbookspider_products.xlsx
+++ b/sportsbook/sportsbookspider_products.xlsx
@@ -14,24 +14,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>轮次</t>
-  </si>
-  <si>
-    <t>时间</t>
-  </si>
-  <si>
-    <t>主隊</t>
-  </si>
-  <si>
-    <t>比分</t>
-  </si>
-  <si>
-    <t>客隊</t>
-  </si>
-  <si>
-    <t>让球</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>比赛Id</t>
+  </si>
+  <si>
+    <t>赛季</t>
+  </si>
+  <si>
+    <t>比赛日</t>
+  </si>
+  <si>
+    <t>比赛时间</t>
+  </si>
+  <si>
+    <t>比赛</t>
+  </si>
+  <si>
+    <t>主队</t>
+  </si>
+  <si>
+    <t>客队</t>
+  </si>
+  <si>
+    <t>主队中文</t>
+  </si>
+  <si>
+    <t>客队中文</t>
+  </si>
+  <si>
+    <t>博彩公司Id</t>
+  </si>
+  <si>
+    <t>博彩公司英文名称</t>
+  </si>
+  <si>
+    <t>博彩公司中文名称</t>
+  </si>
+  <si>
+    <t>初盘主胜赔付</t>
+  </si>
+  <si>
+    <t>初盘平局赔付</t>
+  </si>
+  <si>
+    <t>初盘客胜赔付</t>
+  </si>
+  <si>
+    <t>即时终盘主胜赔付</t>
+  </si>
+  <si>
+    <t>即时终盘平局赔付</t>
+  </si>
+  <si>
+    <t>即时终盘客胜赔付</t>
+  </si>
+  <si>
+    <t>初盘主胜概率</t>
+  </si>
+  <si>
+    <t>即时终盘主胜概率</t>
+  </si>
+  <si>
+    <t>即时终盘平局概率</t>
+  </si>
+  <si>
+    <t>即时终盘客胜概率</t>
   </si>
 </sst>
 </file>
@@ -363,13 +411,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="25" customHeight="1">
+    <row r="1" spans="1:24" ht="25" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,6 +435,60 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sequence of title in excel adjusted
</commit_message>
<xml_diff>
--- a/sportsbook/sportsbookspider_products.xlsx
+++ b/sportsbook/sportsbookspider_products.xlsx
@@ -16,7 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
-    <t>比赛Id</t>
+    <t>联赛名称</t>
+  </si>
+  <si>
+    <t>联赛Id</t>
   </si>
   <si>
     <t>赛季</t>
@@ -26,9 +29,6 @@
   </si>
   <si>
     <t>比赛时间</t>
-  </si>
-  <si>
-    <t>比赛</t>
   </si>
   <si>
     <t>主队</t>

</xml_diff>

<commit_message>
fix export to excel issue!!!
</commit_message>
<xml_diff>
--- a/sportsbook/sportsbookspider_products.xlsx
+++ b/sportsbook/sportsbookspider_products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>联赛名称</t>
   </si>
@@ -34,9 +34,15 @@
     <t>主队</t>
   </si>
   <si>
+    <t>主队排名</t>
+  </si>
+  <si>
     <t>客队</t>
   </si>
   <si>
+    <t>客队排名</t>
+  </si>
+  <si>
     <t>主队中文</t>
   </si>
   <si>
@@ -80,6 +86,165 @@
   </si>
   <si>
     <t>即时终盘客胜概率</t>
+  </si>
+  <si>
+    <t>English Premier League</t>
+  </si>
+  <si>
+    <t>370</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>2017-08-1</t>
+  </si>
+  <si>
+    <t>2017,07-1,28,17,58,00</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Leicester City</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>阿森纳</t>
+  </si>
+  <si>
+    <t>莱切斯特城</t>
+  </si>
+  <si>
+    <t>70283107</t>
+  </si>
+  <si>
+    <t>Oddset</t>
+  </si>
+  <si>
+    <t>Oddset(德国)</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>66.41</t>
+  </si>
+  <si>
+    <t>20.31</t>
+  </si>
+  <si>
+    <t>13.28</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>2017,08-1,11,18,32,00</t>
+  </si>
+  <si>
+    <t>69061424</t>
+  </si>
+  <si>
+    <t>Ladbrokes</t>
+  </si>
+  <si>
+    <t>立博(英国)</t>
+  </si>
+  <si>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>4.33</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>67.38</t>
+  </si>
+  <si>
+    <t>21.16</t>
+  </si>
+  <si>
+    <t>11.45</t>
+  </si>
+  <si>
+    <t>65.21</t>
+  </si>
+  <si>
+    <t>20.75</t>
+  </si>
+  <si>
+    <t>14.04</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>2017,08-1,11,18,40,00</t>
+  </si>
+  <si>
+    <t>69060412</t>
+  </si>
+  <si>
+    <t>William Hill</t>
+  </si>
+  <si>
+    <t>威廉希尔(英国)</t>
+  </si>
+  <si>
+    <t>1.53</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1.44</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>59.52</t>
+  </si>
+  <si>
+    <t>25.3</t>
+  </si>
+  <si>
+    <t>15.18</t>
+  </si>
+  <si>
+    <t>65.54</t>
+  </si>
+  <si>
+    <t>20.97</t>
+  </si>
+  <si>
+    <t>13.48</t>
   </si>
 </sst>
 </file>
@@ -411,13 +576,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="25" customHeight="1">
+    <row r="1" spans="1:26" ht="25" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,19 +641,247 @@
         <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="W1" t="s">
         <v>20</v>
       </c>
       <c r="X1" t="s">
         <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="25" customHeight="1">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="25" customHeight="1">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="25" customHeight="1">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" t="s">
+        <v>70</v>
+      </c>
+      <c r="U4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V4" t="s">
+        <v>72</v>
+      </c>
+      <c r="W4" t="s">
+        <v>73</v>
+      </c>
+      <c r="X4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP asian odds ＋ euro odds export to excel
</commit_message>
<xml_diff>
--- a/sportsbook/sportsbookspider_products.xlsx
+++ b/sportsbook/sportsbookspider_products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>联赛名称</t>
   </si>
@@ -88,6 +88,27 @@
     <t>即时终盘客胜概率</t>
   </si>
   <si>
+    <t>亚盘公司</t>
+  </si>
+  <si>
+    <t>初盘主队水位</t>
+  </si>
+  <si>
+    <t>初盘盘口</t>
+  </si>
+  <si>
+    <t>初盘客队水位</t>
+  </si>
+  <si>
+    <t>即时主队水位</t>
+  </si>
+  <si>
+    <t>即时盘口</t>
+  </si>
+  <si>
+    <t>即时客队水位</t>
+  </si>
+  <si>
     <t>English Premier League</t>
   </si>
   <si>
@@ -146,6 +167,27 @@
   </si>
   <si>
     <t>13.28</t>
+  </si>
+  <si>
+    <t>澳门</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>一球/球半</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>一球</t>
+  </si>
+  <si>
+    <t>1.10</t>
   </si>
   <si>
     <t>82</t>
@@ -576,13 +618,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="25" customHeight="1">
+    <row r="1" spans="1:33" ht="25" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -661,227 +703,311 @@
       <c r="Z1" t="s">
         <v>23</v>
       </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="25" customHeight="1">
+    <row r="2" spans="1:33" ht="25" customHeight="1">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="25" customHeight="1">
+      <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="O2" t="s">
+      <c r="H3" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
+      <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="U2" t="s">
+      <c r="K3" t="s">
         <v>41</v>
       </c>
-      <c r="V2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W2" t="s">
-        <v>43</v>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" t="s">
+        <v>69</v>
+      </c>
+      <c r="W3" t="s">
+        <v>70</v>
+      </c>
+      <c r="X3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="25" customHeight="1">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
+    <row r="4" spans="1:33" ht="25" customHeight="1">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="K3" t="s">
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>81</v>
+      </c>
+      <c r="R4" t="s">
+        <v>82</v>
+      </c>
+      <c r="S4" t="s">
+        <v>83</v>
+      </c>
+      <c r="T4" t="s">
+        <v>84</v>
+      </c>
+      <c r="U4" t="s">
+        <v>85</v>
+      </c>
+      <c r="V4" t="s">
+        <v>86</v>
+      </c>
+      <c r="W4" t="s">
+        <v>87</v>
+      </c>
+      <c r="X4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA4" t="s">
         <v>51</v>
       </c>
-      <c r="R3" t="s">
+      <c r="AB4" t="s">
         <v>52</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AC4" t="s">
         <v>53</v>
       </c>
-      <c r="T3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="AD4" t="s">
         <v>54</v>
       </c>
-      <c r="V3" t="s">
+      <c r="AE4" t="s">
         <v>55</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AF4" t="s">
         <v>56</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AG4" t="s">
         <v>57</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="25" customHeight="1">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>67</v>
-      </c>
-      <c r="R4" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" t="s">
-        <v>70</v>
-      </c>
-      <c r="U4" t="s">
-        <v>71</v>
-      </c>
-      <c r="V4" t="s">
-        <v>72</v>
-      </c>
-      <c r="W4" t="s">
-        <v>73</v>
-      </c>
-      <c r="X4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>